<commit_message>
Added multi line matching. Made it so orders always are shown in the GUI
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/gingoso2@gmail.com_CLEAVE.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/gingoso2@gmail.com_CLEAVE.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,18 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3 cases extra thin ravioli sheets</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3 RAVSHE 4E</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>